<commit_message>
call of cthulhu product_code
</commit_message>
<xml_diff>
--- a/call-of-cthulhu/checklist.xlsx
+++ b/call-of-cthulhu/checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/call-of-cthulhu/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6698058B-CE87-2D49-ACC2-A1B77AEE4FAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B83463-50E1-694D-96D2-549EA6F65F54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="18740" xr2:uid="{4232880B-E93C-A846-8BEC-E451E9244CE3}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" xr2:uid="{4232880B-E93C-A846-8BEC-E451E9244CE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="68">
   <si>
     <t>year</t>
   </si>
@@ -201,6 +201,42 @@
   </si>
   <si>
     <t>cthulhu_world_tour.jpg</t>
+  </si>
+  <si>
+    <t>product_code</t>
+  </si>
+  <si>
+    <t>No. 128</t>
+  </si>
+  <si>
+    <t>No. 128-2</t>
+  </si>
+  <si>
+    <t>No. 128-8</t>
+  </si>
+  <si>
+    <t>No. 128-6</t>
+  </si>
+  <si>
+    <t>No. 128-1</t>
+  </si>
+  <si>
+    <t>No. 128-4</t>
+  </si>
+  <si>
+    <t>No. 128-3</t>
+  </si>
+  <si>
+    <t>No. 128-7</t>
+  </si>
+  <si>
+    <t>No. 128-10</t>
+  </si>
+  <si>
+    <t>No. 128-5</t>
+  </si>
+  <si>
+    <t>No. 128-9</t>
   </si>
 </sst>
 </file>
@@ -561,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB5384AA-C9B0-9948-A0FD-C5F2BA8A2AE3}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -573,9 +609,10 @@
     <col min="3" max="3" width="62" customWidth="1"/>
     <col min="4" max="4" width="28.5" customWidth="1"/>
     <col min="5" max="5" width="32.1640625" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -594,8 +631,11 @@
       <c r="F1" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>48</v>
       </c>
@@ -611,8 +651,11 @@
       <c r="F2" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>46</v>
       </c>
@@ -628,8 +671,11 @@
       <c r="F3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1986</v>
       </c>
@@ -648,8 +694,11 @@
       <c r="F4" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>22</v>
       </c>
@@ -666,7 +715,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>34</v>
       </c>
@@ -682,8 +731,11 @@
       <c r="F6" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>36</v>
       </c>
@@ -699,8 +751,11 @@
       <c r="F7" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>40</v>
       </c>
@@ -717,7 +772,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>44</v>
       </c>
@@ -734,7 +789,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>42</v>
       </c>
@@ -751,7 +806,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>24</v>
       </c>
@@ -767,8 +822,11 @@
       <c r="F11" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1990</v>
       </c>
@@ -788,7 +846,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>27</v>
       </c>
@@ -804,8 +862,11 @@
       <c r="F13" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>38</v>
       </c>
@@ -821,8 +882,11 @@
       <c r="F14" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>26</v>
       </c>
@@ -838,8 +902,11 @@
       <c r="F15" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>32</v>
       </c>
@@ -855,8 +922,11 @@
       <c r="F16" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>30</v>
       </c>
@@ -871,6 +941,9 @@
       </c>
       <c r="F17" t="s">
         <v>52</v>
+      </c>
+      <c r="G17" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>